<commit_message>
Table 2 - completed summary statistics
</commit_message>
<xml_diff>
--- a/table_outputs.xlsx
+++ b/table_outputs.xlsx
@@ -9,12 +9,14 @@
     <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Table 1" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Table 2 - circle" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Table 2 - city" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Table 2 - country" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="221">
   <si>
     <t xml:space="preserve">country</t>
   </si>
@@ -626,6 +628,57 @@
   </si>
   <si>
     <t xml:space="preserve">6.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 (33%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 (1.00)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 (0.00)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 (0.50)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31 (22%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">71 (59%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 (1.00)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">53 (23%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17 (40%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32 (53%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 (2.25)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">66 (72%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">72%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 (2.00)</t>
   </si>
 </sst>
 </file>
@@ -2186,4 +2239,342 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>204</v>
+      </c>
+      <c r="E2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2" t="s">
+        <v>205</v>
+      </c>
+      <c r="G2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" t="s">
+        <v>206</v>
+      </c>
+      <c r="G3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" t="s">
+        <v>207</v>
+      </c>
+      <c r="G4" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" t="s">
+        <v>209</v>
+      </c>
+      <c r="E5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" t="s">
+        <v>206</v>
+      </c>
+      <c r="G5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" t="s">
+        <v>210</v>
+      </c>
+      <c r="E6" t="s">
+        <v>193</v>
+      </c>
+      <c r="F6" t="s">
+        <v>211</v>
+      </c>
+      <c r="G6" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" t="s">
+        <v>212</v>
+      </c>
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" t="s">
+        <v>206</v>
+      </c>
+      <c r="G7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D8" t="s">
+        <v>213</v>
+      </c>
+      <c r="E8" t="s">
+        <v>214</v>
+      </c>
+      <c r="F8" t="s">
+        <v>205</v>
+      </c>
+      <c r="G8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>215</v>
+      </c>
+      <c r="E9" t="s">
+        <v>116</v>
+      </c>
+      <c r="F9" t="s">
+        <v>216</v>
+      </c>
+      <c r="G9" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D10" t="s">
+        <v>218</v>
+      </c>
+      <c r="E10" t="s">
+        <v>219</v>
+      </c>
+      <c r="F10" t="s">
+        <v>220</v>
+      </c>
+      <c r="G10" t="s">
+        <v>186</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="n">
+        <v>126</v>
+      </c>
+      <c r="C2" t="n">
+        <v>26</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.206349206349206</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" t="n">
+        <v>487</v>
+      </c>
+      <c r="C3" t="n">
+        <v>155</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.318275154004107</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" t="n">
+        <v>195</v>
+      </c>
+      <c r="C4" t="n">
+        <v>115</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.58974358974359</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" t="n">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Export rice price data
</commit_message>
<xml_diff>
--- a/table_outputs.xlsx
+++ b/table_outputs.xlsx
@@ -1,692 +1,699 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr date1904="false"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s1985751\Documents\GitHub\fea\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F03EFDAE-F097-486C-93F5-91D977EDBB34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Table 1" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Table 2 - circle" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Table 2 - city" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Table 2 - country" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Table 1" sheetId="2" r:id="rId2"/>
+    <sheet name="Table 2 - circle" sheetId="3" r:id="rId3"/>
+    <sheet name="Table 2 - city" sheetId="4" r:id="rId4"/>
+    <sheet name="Table 2 - country" sheetId="5" r:id="rId5"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="221">
-  <si>
-    <t xml:space="preserve">country</t>
-  </si>
-  <si>
-    <t xml:space="preserve">city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">total_vendors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Higher</t>
-  </si>
-  <si>
-    <t xml:space="preserve">higher_perc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Middle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">middle_perc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lower</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lower_perc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mobile vendor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mobile_vendor_perc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stationary small local vendor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stationary_small_vendor_perc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supermarket</t>
-  </si>
-  <si>
-    <t xml:space="preserve">supermarket_perc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brazil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rio de Janeiro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">60</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14 (23%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18 (30%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28 (47%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">47%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 (2%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">42 (70%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">70%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17 (28%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sao Paolo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">58</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 (7%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">41 (71%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">71%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13 (22%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0 (0%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50 (86%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">86%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8 (14%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sinop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 (25%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 (50%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 (12%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7 (88%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">88%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">India</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hyderabad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">141</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25 (18%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22 (16%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">94 (67%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">67%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15 (11%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">120 (85%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">85%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 (4%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Latur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">120</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16 (13%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30 (25%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">74 (62%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">62%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11 (9%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">108 (90%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">90%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 (1%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Visakhapatnam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">226</t>
-  </si>
-  <si>
-    <t xml:space="preserve">103 (46%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">46%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">54 (24%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">69 (31%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">31%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30 (13%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">176 (78%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">78%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20 (9%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Birmingham</t>
-  </si>
-  <si>
-    <t xml:space="preserve">43</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11 (26%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19 (44%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">44%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13 (30%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29 (67%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14 (33%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">33%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Edinburgh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15 (25%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29 (48%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">48%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16 (27%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">45 (75%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">75%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">London</t>
-  </si>
-  <si>
-    <t xml:space="preserve">92</t>
-  </si>
-  <si>
-    <t xml:space="preserve">49 (53%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">53%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30 (33%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13 (14%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 (7%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">69 (75%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17 (18%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">circle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vendors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">count_org_vendors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">org_vendor_perc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">median_org_foods_count</t>
-  </si>
-  <si>
-    <t xml:space="preserve">iqr_org_foods_count</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11 (79%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">79%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.0 (4.75)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.75</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5 (28%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0 (0.75)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.75</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 (14%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0 (0.00)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 (50%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.0 (4.50)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">41</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 (8%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 (50%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.0 (3.00)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.0 (1.00)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9 (36%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">36%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0 (1.00)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11 (50%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.5 (1.00)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">94</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11 (12%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9 (56%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">56%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21 (70%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">74</t>
-  </si>
-  <si>
-    <t xml:space="preserve">41 (55%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">55%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">103</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19 (18%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">54</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22 (41%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">41%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">69</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12 (17%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 (55%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.0 (3.00)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9 (47%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0 (2.00)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 (15%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7 (47%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17 (59%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">59%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8 (50%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.5 (2.00)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">49</t>
-  </si>
-  <si>
-    <t xml:space="preserve">32 (65%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">65%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.0 (2.00)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13 (100%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.0 (6.00)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20 (33%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0 (1.00)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0 (0.00)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0 (0.50)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">31 (22%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">71 (59%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 (1.00)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">53 (23%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17 (40%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">40%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">32 (53%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 (2.25)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">66 (72%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">72%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 (2.00)</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="221">
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>total_vendors</t>
+  </si>
+  <si>
+    <t>Higher</t>
+  </si>
+  <si>
+    <t>higher_perc</t>
+  </si>
+  <si>
+    <t>Middle</t>
+  </si>
+  <si>
+    <t>middle_perc</t>
+  </si>
+  <si>
+    <t>Lower</t>
+  </si>
+  <si>
+    <t>lower_perc</t>
+  </si>
+  <si>
+    <t>Mobile vendor</t>
+  </si>
+  <si>
+    <t>mobile_vendor_perc</t>
+  </si>
+  <si>
+    <t>Stationary small local vendor</t>
+  </si>
+  <si>
+    <t>stationary_small_vendor_perc</t>
+  </si>
+  <si>
+    <t>Supermarket</t>
+  </si>
+  <si>
+    <t>supermarket_perc</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>Rio de Janeiro</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>14 (23%)</t>
+  </si>
+  <si>
+    <t>23%</t>
+  </si>
+  <si>
+    <t>18 (30%)</t>
+  </si>
+  <si>
+    <t>30%</t>
+  </si>
+  <si>
+    <t>28 (47%)</t>
+  </si>
+  <si>
+    <t>47%</t>
+  </si>
+  <si>
+    <t>1 (2%)</t>
+  </si>
+  <si>
+    <t>2%</t>
+  </si>
+  <si>
+    <t>42 (70%)</t>
+  </si>
+  <si>
+    <t>70%</t>
+  </si>
+  <si>
+    <t>17 (28%)</t>
+  </si>
+  <si>
+    <t>28%</t>
+  </si>
+  <si>
+    <t>Sao Paolo</t>
+  </si>
+  <si>
+    <t>58</t>
+  </si>
+  <si>
+    <t>4 (7%)</t>
+  </si>
+  <si>
+    <t>7%</t>
+  </si>
+  <si>
+    <t>41 (71%)</t>
+  </si>
+  <si>
+    <t>71%</t>
+  </si>
+  <si>
+    <t>13 (22%)</t>
+  </si>
+  <si>
+    <t>22%</t>
+  </si>
+  <si>
+    <t>0 (0%)</t>
+  </si>
+  <si>
+    <t>0%</t>
+  </si>
+  <si>
+    <t>50 (86%)</t>
+  </si>
+  <si>
+    <t>86%</t>
+  </si>
+  <si>
+    <t>8 (14%)</t>
+  </si>
+  <si>
+    <t>14%</t>
+  </si>
+  <si>
+    <t>Sinop</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>2 (25%)</t>
+  </si>
+  <si>
+    <t>25%</t>
+  </si>
+  <si>
+    <t>4 (50%)</t>
+  </si>
+  <si>
+    <t>50%</t>
+  </si>
+  <si>
+    <t>1 (12%)</t>
+  </si>
+  <si>
+    <t>12%</t>
+  </si>
+  <si>
+    <t>7 (88%)</t>
+  </si>
+  <si>
+    <t>88%</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Hyderabad</t>
+  </si>
+  <si>
+    <t>141</t>
+  </si>
+  <si>
+    <t>25 (18%)</t>
+  </si>
+  <si>
+    <t>18%</t>
+  </si>
+  <si>
+    <t>22 (16%)</t>
+  </si>
+  <si>
+    <t>16%</t>
+  </si>
+  <si>
+    <t>94 (67%)</t>
+  </si>
+  <si>
+    <t>67%</t>
+  </si>
+  <si>
+    <t>15 (11%)</t>
+  </si>
+  <si>
+    <t>11%</t>
+  </si>
+  <si>
+    <t>120 (85%)</t>
+  </si>
+  <si>
+    <t>85%</t>
+  </si>
+  <si>
+    <t>6 (4%)</t>
+  </si>
+  <si>
+    <t>4%</t>
+  </si>
+  <si>
+    <t>Latur</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t>16 (13%)</t>
+  </si>
+  <si>
+    <t>13%</t>
+  </si>
+  <si>
+    <t>30 (25%)</t>
+  </si>
+  <si>
+    <t>74 (62%)</t>
+  </si>
+  <si>
+    <t>62%</t>
+  </si>
+  <si>
+    <t>11 (9%)</t>
+  </si>
+  <si>
+    <t>9%</t>
+  </si>
+  <si>
+    <t>108 (90%)</t>
+  </si>
+  <si>
+    <t>90%</t>
+  </si>
+  <si>
+    <t>1 (1%)</t>
+  </si>
+  <si>
+    <t>1%</t>
+  </si>
+  <si>
+    <t>Visakhapatnam</t>
+  </si>
+  <si>
+    <t>226</t>
+  </si>
+  <si>
+    <t>103 (46%)</t>
+  </si>
+  <si>
+    <t>46%</t>
+  </si>
+  <si>
+    <t>54 (24%)</t>
+  </si>
+  <si>
+    <t>24%</t>
+  </si>
+  <si>
+    <t>69 (31%)</t>
+  </si>
+  <si>
+    <t>31%</t>
+  </si>
+  <si>
+    <t>30 (13%)</t>
+  </si>
+  <si>
+    <t>176 (78%)</t>
+  </si>
+  <si>
+    <t>78%</t>
+  </si>
+  <si>
+    <t>20 (9%)</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>Birmingham</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>11 (26%)</t>
+  </si>
+  <si>
+    <t>26%</t>
+  </si>
+  <si>
+    <t>19 (44%)</t>
+  </si>
+  <si>
+    <t>44%</t>
+  </si>
+  <si>
+    <t>13 (30%)</t>
+  </si>
+  <si>
+    <t>29 (67%)</t>
+  </si>
+  <si>
+    <t>14 (33%)</t>
+  </si>
+  <si>
+    <t>33%</t>
+  </si>
+  <si>
+    <t>Edinburgh</t>
+  </si>
+  <si>
+    <t>15 (25%)</t>
+  </si>
+  <si>
+    <t>29 (48%)</t>
+  </si>
+  <si>
+    <t>48%</t>
+  </si>
+  <si>
+    <t>16 (27%)</t>
+  </si>
+  <si>
+    <t>27%</t>
+  </si>
+  <si>
+    <t>45 (75%)</t>
+  </si>
+  <si>
+    <t>75%</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>92</t>
+  </si>
+  <si>
+    <t>49 (53%)</t>
+  </si>
+  <si>
+    <t>53%</t>
+  </si>
+  <si>
+    <t>30 (33%)</t>
+  </si>
+  <si>
+    <t>13 (14%)</t>
+  </si>
+  <si>
+    <t>6 (7%)</t>
+  </si>
+  <si>
+    <t>69 (75%)</t>
+  </si>
+  <si>
+    <t>17 (18%)</t>
+  </si>
+  <si>
+    <t>circle</t>
+  </si>
+  <si>
+    <t>vendors</t>
+  </si>
+  <si>
+    <t>count_org_vendors</t>
+  </si>
+  <si>
+    <t>org_vendor_perc</t>
+  </si>
+  <si>
+    <t>median_org_foods_count</t>
+  </si>
+  <si>
+    <t>iqr_org_foods_count</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>11 (79%)</t>
+  </si>
+  <si>
+    <t>79%</t>
+  </si>
+  <si>
+    <t>4.0 (4.75)</t>
+  </si>
+  <si>
+    <t>4.75</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>5 (28%)</t>
+  </si>
+  <si>
+    <t>0.0 (0.75)</t>
+  </si>
+  <si>
+    <t>0.75</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>4 (14%)</t>
+  </si>
+  <si>
+    <t>0.0 (0.00)</t>
+  </si>
+  <si>
+    <t>0.00</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>2 (50%)</t>
+  </si>
+  <si>
+    <t>1.0 (4.50)</t>
+  </si>
+  <si>
+    <t>4.50</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>1 (8%)</t>
+  </si>
+  <si>
+    <t>8%</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>1 (50%)</t>
+  </si>
+  <si>
+    <t>3.0 (3.00)</t>
+  </si>
+  <si>
+    <t>3.00</t>
+  </si>
+  <si>
+    <t>1.0 (1.00)</t>
+  </si>
+  <si>
+    <t>1.00</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>9 (36%)</t>
+  </si>
+  <si>
+    <t>36%</t>
+  </si>
+  <si>
+    <t>0.0 (1.00)</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>11 (50%)</t>
+  </si>
+  <si>
+    <t>0.5 (1.00)</t>
+  </si>
+  <si>
+    <t>94</t>
+  </si>
+  <si>
+    <t>11 (12%)</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>9 (56%)</t>
+  </si>
+  <si>
+    <t>56%</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>21 (70%)</t>
+  </si>
+  <si>
+    <t>74</t>
+  </si>
+  <si>
+    <t>41 (55%)</t>
+  </si>
+  <si>
+    <t>55%</t>
+  </si>
+  <si>
+    <t>103</t>
+  </si>
+  <si>
+    <t>19 (18%)</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>22 (41%)</t>
+  </si>
+  <si>
+    <t>41%</t>
+  </si>
+  <si>
+    <t>69</t>
+  </si>
+  <si>
+    <t>12 (17%)</t>
+  </si>
+  <si>
+    <t>17%</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>6 (55%)</t>
+  </si>
+  <si>
+    <t>1.0 (3.00)</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>9 (47%)</t>
+  </si>
+  <si>
+    <t>0.0 (2.00)</t>
+  </si>
+  <si>
+    <t>2.00</t>
+  </si>
+  <si>
+    <t>2 (15%)</t>
+  </si>
+  <si>
+    <t>15%</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>7 (47%)</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>17 (59%)</t>
+  </si>
+  <si>
+    <t>59%</t>
+  </si>
+  <si>
+    <t>8 (50%)</t>
+  </si>
+  <si>
+    <t>0.5 (2.00)</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>32 (65%)</t>
+  </si>
+  <si>
+    <t>65%</t>
+  </si>
+  <si>
+    <t>1.0 (2.00)</t>
+  </si>
+  <si>
+    <t>13 (100%)</t>
+  </si>
+  <si>
+    <t>100%</t>
+  </si>
+  <si>
+    <t>3.0 (6.00)</t>
+  </si>
+  <si>
+    <t>6.00</t>
+  </si>
+  <si>
+    <t>20 (33%)</t>
+  </si>
+  <si>
+    <t>0 (1.00)</t>
+  </si>
+  <si>
+    <t>0 (0.00)</t>
+  </si>
+  <si>
+    <t>0 (0.50)</t>
+  </si>
+  <si>
+    <t>0.50</t>
+  </si>
+  <si>
+    <t>31 (22%)</t>
+  </si>
+  <si>
+    <t>71 (59%)</t>
+  </si>
+  <si>
+    <t>1 (1.00)</t>
+  </si>
+  <si>
+    <t>53 (23%)</t>
+  </si>
+  <si>
+    <t>17 (40%)</t>
+  </si>
+  <si>
+    <t>40%</t>
+  </si>
+  <si>
+    <t>32 (53%)</t>
+  </si>
+  <si>
+    <t>1 (2.25)</t>
+  </si>
+  <si>
+    <t>2.25</t>
+  </si>
+  <si>
+    <t>66 (72%)</t>
+  </si>
+  <si>
+    <t>72%</t>
+  </si>
+  <si>
+    <t>1 (2.00)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -722,6 +729,15 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1003,27 +1019,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="NA" tabSelected="true"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1070,7 +1086,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1117,7 +1133,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1164,7 +1180,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1211,7 +1227,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>54</v>
       </c>
@@ -1258,7 +1274,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>54</v>
       </c>
@@ -1305,7 +1321,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>54</v>
       </c>
@@ -1352,7 +1368,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>94</v>
       </c>
@@ -1399,7 +1415,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>94</v>
       </c>
@@ -1446,7 +1462,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>94</v>
       </c>
@@ -1495,19 +1511,19 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1533,7 +1549,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1559,7 +1575,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1585,7 +1601,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1611,7 +1627,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1637,7 +1653,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1663,7 +1679,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1689,7 +1705,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1715,7 +1731,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1741,7 +1757,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -1767,7 +1783,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>54</v>
       </c>
@@ -1793,7 +1809,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>54</v>
       </c>
@@ -1819,7 +1835,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>54</v>
       </c>
@@ -1845,7 +1861,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>54</v>
       </c>
@@ -1871,7 +1887,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>54</v>
       </c>
@@ -1897,7 +1913,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -1923,7 +1939,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>54</v>
       </c>
@@ -1949,7 +1965,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>54</v>
       </c>
@@ -1975,7 +1991,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>54</v>
       </c>
@@ -2001,7 +2017,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>94</v>
       </c>
@@ -2027,7 +2043,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>94</v>
       </c>
@@ -2053,7 +2069,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>94</v>
       </c>
@@ -2079,7 +2095,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>94</v>
       </c>
@@ -2105,7 +2121,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>94</v>
       </c>
@@ -2131,7 +2147,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>94</v>
       </c>
@@ -2157,7 +2173,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>94</v>
       </c>
@@ -2183,7 +2199,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>94</v>
       </c>
@@ -2209,7 +2225,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>94</v>
       </c>
@@ -2237,19 +2253,21 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2272,7 +2290,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -2295,7 +2313,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -2318,7 +2336,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -2341,7 +2359,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>54</v>
       </c>
@@ -2364,7 +2382,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>54</v>
       </c>
@@ -2387,7 +2405,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>54</v>
       </c>
@@ -2410,7 +2428,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>94</v>
       </c>
@@ -2433,7 +2451,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>94</v>
       </c>
@@ -2456,7 +2474,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>94</v>
       </c>
@@ -2481,19 +2499,19 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2513,68 +2531,68 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2">
         <v>126</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>26</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2">
         <v>0.206349206349206</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2">
         <v>0</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F2">
         <v>0</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>54</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>487</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>155</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3">
         <v>0.318275154004107</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E3">
         <v>0</v>
       </c>
-      <c r="F3" t="n">
+      <c r="F3">
         <v>1</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>94</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4">
         <v>195</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4">
         <v>115</v>
       </c>
-      <c r="D4" t="n">
-        <v>0.58974358974359</v>
-      </c>
-      <c r="E4" t="n">
+      <c r="D4">
+        <v>0.58974358974358998</v>
+      </c>
+      <c r="E4">
         <v>1</v>
       </c>
-      <c r="F4" t="n">
+      <c r="F4">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cleaning up and exporting Tables
</commit_message>
<xml_diff>
--- a/table_outputs.xlsx
+++ b/table_outputs.xlsx
@@ -9,12 +9,18 @@
     <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Table 1" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Table 2" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Table 2 - neighbourhood" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Table 2 - city" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Table 2 - country" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Table 3 - neighbourhood" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Table 3 - city" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Table 3 - country" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="226">
   <si>
     <t xml:space="preserve">country</t>
   </si>
@@ -626,6 +632,72 @@
   </si>
   <si>
     <t xml:space="preserve">6.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 (33%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 (1.00)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 (0.00)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 (0.50)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31 (22%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">71 (59%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 (1.00)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">53 (23%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17 (40%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32 (53%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 (2.25)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">66 (72%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">72%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 (2.00)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">organic_vendors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n_multiple_org_binary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">perc_multiple_org_binary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">median_multiple_org_count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iqr_multiple_org_count</t>
   </si>
 </sst>
 </file>
@@ -2186,4 +2258,2164 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G1" t="s">
+        <v>126</v>
+      </c>
+      <c r="H1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2" t="s">
+        <v>130</v>
+      </c>
+      <c r="G2" t="s">
+        <v>131</v>
+      </c>
+      <c r="H2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E3" t="s">
+        <v>134</v>
+      </c>
+      <c r="F3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" t="s">
+        <v>135</v>
+      </c>
+      <c r="H3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E4" t="s">
+        <v>138</v>
+      </c>
+      <c r="F4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" t="s">
+        <v>139</v>
+      </c>
+      <c r="H4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>141</v>
+      </c>
+      <c r="E5" t="s">
+        <v>142</v>
+      </c>
+      <c r="F5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" t="s">
+        <v>143</v>
+      </c>
+      <c r="H5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>145</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" t="s">
+        <v>139</v>
+      </c>
+      <c r="H6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>146</v>
+      </c>
+      <c r="E7" t="s">
+        <v>147</v>
+      </c>
+      <c r="F7" t="s">
+        <v>148</v>
+      </c>
+      <c r="G7" t="s">
+        <v>139</v>
+      </c>
+      <c r="H7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>149</v>
+      </c>
+      <c r="E8" t="s">
+        <v>150</v>
+      </c>
+      <c r="F8" t="s">
+        <v>49</v>
+      </c>
+      <c r="G8" t="s">
+        <v>151</v>
+      </c>
+      <c r="H8" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>149</v>
+      </c>
+      <c r="E9" t="s">
+        <v>150</v>
+      </c>
+      <c r="F9" t="s">
+        <v>49</v>
+      </c>
+      <c r="G9" t="s">
+        <v>153</v>
+      </c>
+      <c r="H9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>141</v>
+      </c>
+      <c r="E10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" t="s">
+        <v>139</v>
+      </c>
+      <c r="H10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>155</v>
+      </c>
+      <c r="E11" t="s">
+        <v>156</v>
+      </c>
+      <c r="F11" t="s">
+        <v>157</v>
+      </c>
+      <c r="G11" t="s">
+        <v>158</v>
+      </c>
+      <c r="H11" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>159</v>
+      </c>
+      <c r="E12" t="s">
+        <v>160</v>
+      </c>
+      <c r="F12" t="s">
+        <v>49</v>
+      </c>
+      <c r="G12" t="s">
+        <v>161</v>
+      </c>
+      <c r="H12" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" t="s">
+        <v>162</v>
+      </c>
+      <c r="E13" t="s">
+        <v>163</v>
+      </c>
+      <c r="F13" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" t="s">
+        <v>139</v>
+      </c>
+      <c r="H13" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" t="s">
+        <v>164</v>
+      </c>
+      <c r="E14" t="s">
+        <v>165</v>
+      </c>
+      <c r="F14" t="s">
+        <v>166</v>
+      </c>
+      <c r="G14" t="s">
+        <v>153</v>
+      </c>
+      <c r="H14" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>167</v>
+      </c>
+      <c r="E15" t="s">
+        <v>168</v>
+      </c>
+      <c r="F15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15" t="s">
+        <v>153</v>
+      </c>
+      <c r="H15" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" t="s">
+        <v>169</v>
+      </c>
+      <c r="E16" t="s">
+        <v>170</v>
+      </c>
+      <c r="F16" t="s">
+        <v>171</v>
+      </c>
+      <c r="G16" t="s">
+        <v>153</v>
+      </c>
+      <c r="H16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" t="s">
+        <v>172</v>
+      </c>
+      <c r="E17" t="s">
+        <v>173</v>
+      </c>
+      <c r="F17" t="s">
+        <v>58</v>
+      </c>
+      <c r="G17" t="s">
+        <v>139</v>
+      </c>
+      <c r="H17" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s">
+        <v>174</v>
+      </c>
+      <c r="E18" t="s">
+        <v>175</v>
+      </c>
+      <c r="F18" t="s">
+        <v>176</v>
+      </c>
+      <c r="G18" t="s">
+        <v>158</v>
+      </c>
+      <c r="H18" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" t="s">
+        <v>177</v>
+      </c>
+      <c r="E19" t="s">
+        <v>178</v>
+      </c>
+      <c r="F19" t="s">
+        <v>179</v>
+      </c>
+      <c r="G19" t="s">
+        <v>139</v>
+      </c>
+      <c r="H19" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>94</v>
+      </c>
+      <c r="B20" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" t="s">
+        <v>180</v>
+      </c>
+      <c r="E20" t="s">
+        <v>181</v>
+      </c>
+      <c r="F20" t="s">
+        <v>171</v>
+      </c>
+      <c r="G20" t="s">
+        <v>182</v>
+      </c>
+      <c r="H20" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>94</v>
+      </c>
+      <c r="B21" t="s">
+        <v>95</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" t="s">
+        <v>183</v>
+      </c>
+      <c r="E21" t="s">
+        <v>184</v>
+      </c>
+      <c r="F21" t="s">
+        <v>23</v>
+      </c>
+      <c r="G21" t="s">
+        <v>185</v>
+      </c>
+      <c r="H21" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>94</v>
+      </c>
+      <c r="B22" t="s">
+        <v>95</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" t="s">
+        <v>146</v>
+      </c>
+      <c r="E22" t="s">
+        <v>187</v>
+      </c>
+      <c r="F22" t="s">
+        <v>188</v>
+      </c>
+      <c r="G22" t="s">
+        <v>139</v>
+      </c>
+      <c r="H22" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>94</v>
+      </c>
+      <c r="B23" t="s">
+        <v>105</v>
+      </c>
+      <c r="C23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" t="s">
+        <v>189</v>
+      </c>
+      <c r="E23" t="s">
+        <v>190</v>
+      </c>
+      <c r="F23" t="s">
+        <v>23</v>
+      </c>
+      <c r="G23" t="s">
+        <v>185</v>
+      </c>
+      <c r="H23" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>94</v>
+      </c>
+      <c r="B24" t="s">
+        <v>105</v>
+      </c>
+      <c r="C24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" t="s">
+        <v>191</v>
+      </c>
+      <c r="E24" t="s">
+        <v>192</v>
+      </c>
+      <c r="F24" t="s">
+        <v>193</v>
+      </c>
+      <c r="G24" t="s">
+        <v>182</v>
+      </c>
+      <c r="H24" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>94</v>
+      </c>
+      <c r="B25" t="s">
+        <v>105</v>
+      </c>
+      <c r="C25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" t="s">
+        <v>164</v>
+      </c>
+      <c r="E25" t="s">
+        <v>194</v>
+      </c>
+      <c r="F25" t="s">
+        <v>49</v>
+      </c>
+      <c r="G25" t="s">
+        <v>195</v>
+      </c>
+      <c r="H25" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>94</v>
+      </c>
+      <c r="B26" t="s">
+        <v>113</v>
+      </c>
+      <c r="C26" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" t="s">
+        <v>196</v>
+      </c>
+      <c r="E26" t="s">
+        <v>197</v>
+      </c>
+      <c r="F26" t="s">
+        <v>198</v>
+      </c>
+      <c r="G26" t="s">
+        <v>199</v>
+      </c>
+      <c r="H26" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>94</v>
+      </c>
+      <c r="B27" t="s">
+        <v>113</v>
+      </c>
+      <c r="C27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" t="s">
+        <v>167</v>
+      </c>
+      <c r="E27" t="s">
+        <v>168</v>
+      </c>
+      <c r="F27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G27" t="s">
+        <v>153</v>
+      </c>
+      <c r="H27" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>94</v>
+      </c>
+      <c r="B28" t="s">
+        <v>113</v>
+      </c>
+      <c r="C28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" t="s">
+        <v>146</v>
+      </c>
+      <c r="E28" t="s">
+        <v>200</v>
+      </c>
+      <c r="F28" t="s">
+        <v>201</v>
+      </c>
+      <c r="G28" t="s">
+        <v>202</v>
+      </c>
+      <c r="H28" t="s">
+        <v>203</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>204</v>
+      </c>
+      <c r="E2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2" t="s">
+        <v>205</v>
+      </c>
+      <c r="G2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" t="s">
+        <v>206</v>
+      </c>
+      <c r="G3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" t="s">
+        <v>207</v>
+      </c>
+      <c r="G4" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" t="s">
+        <v>209</v>
+      </c>
+      <c r="E5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" t="s">
+        <v>206</v>
+      </c>
+      <c r="G5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" t="s">
+        <v>210</v>
+      </c>
+      <c r="E6" t="s">
+        <v>193</v>
+      </c>
+      <c r="F6" t="s">
+        <v>211</v>
+      </c>
+      <c r="G6" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" t="s">
+        <v>212</v>
+      </c>
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" t="s">
+        <v>206</v>
+      </c>
+      <c r="G7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D8" t="s">
+        <v>213</v>
+      </c>
+      <c r="E8" t="s">
+        <v>214</v>
+      </c>
+      <c r="F8" t="s">
+        <v>205</v>
+      </c>
+      <c r="G8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>215</v>
+      </c>
+      <c r="E9" t="s">
+        <v>116</v>
+      </c>
+      <c r="F9" t="s">
+        <v>216</v>
+      </c>
+      <c r="G9" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D10" t="s">
+        <v>218</v>
+      </c>
+      <c r="E10" t="s">
+        <v>219</v>
+      </c>
+      <c r="F10" t="s">
+        <v>220</v>
+      </c>
+      <c r="G10" t="s">
+        <v>186</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="n">
+        <v>126</v>
+      </c>
+      <c r="C2" t="n">
+        <v>26</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.206349206349206</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" t="n">
+        <v>487</v>
+      </c>
+      <c r="C3" t="n">
+        <v>155</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.318275154004107</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" t="n">
+        <v>195</v>
+      </c>
+      <c r="C4" t="n">
+        <v>115</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.58974358974359</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" t="n">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D1" t="s">
+        <v>221</v>
+      </c>
+      <c r="E1" t="s">
+        <v>222</v>
+      </c>
+      <c r="F1" t="s">
+        <v>223</v>
+      </c>
+      <c r="G1" t="s">
+        <v>224</v>
+      </c>
+      <c r="H1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="n">
+        <v>11</v>
+      </c>
+      <c r="E2" t="n">
+        <v>10</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.909090909090909</v>
+      </c>
+      <c r="G2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" t="n">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="n">
+        <v>5</v>
+      </c>
+      <c r="E3" t="n">
+        <v>3</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="n">
+        <v>4</v>
+      </c>
+      <c r="E4" t="n">
+        <v>3</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" t="n">
+        <v>2</v>
+      </c>
+      <c r="E5" t="n">
+        <v>2</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" t="n">
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" t="n">
+        <v>2</v>
+      </c>
+      <c r="H8" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" t="n">
+        <v>9</v>
+      </c>
+      <c r="E11" t="n">
+        <v>5</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.555555555555556</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="n">
+        <v>11</v>
+      </c>
+      <c r="E12" t="n">
+        <v>2</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.181818181818182</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" t="n">
+        <v>11</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" t="n">
+        <v>9</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.111111111111111</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" t="n">
+        <v>21</v>
+      </c>
+      <c r="E15" t="n">
+        <v>2</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.0952380952380952</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" t="n">
+        <v>41</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" t="n">
+        <v>19</v>
+      </c>
+      <c r="E17" t="n">
+        <v>10</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.526315789473684</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" t="n">
+        <v>22</v>
+      </c>
+      <c r="E18" t="n">
+        <v>13</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.590909090909091</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" t="n">
+        <v>12</v>
+      </c>
+      <c r="E19" t="n">
+        <v>6</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>94</v>
+      </c>
+      <c r="B20" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" t="n">
+        <v>6</v>
+      </c>
+      <c r="E20" t="n">
+        <v>3</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>94</v>
+      </c>
+      <c r="B21" t="s">
+        <v>95</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" t="n">
+        <v>9</v>
+      </c>
+      <c r="E21" t="n">
+        <v>6</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>94</v>
+      </c>
+      <c r="B22" t="s">
+        <v>95</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" t="n">
+        <v>2</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>94</v>
+      </c>
+      <c r="B23" t="s">
+        <v>105</v>
+      </c>
+      <c r="C23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" t="n">
+        <v>7</v>
+      </c>
+      <c r="E23" t="n">
+        <v>4</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.571428571428571</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>94</v>
+      </c>
+      <c r="B24" t="s">
+        <v>105</v>
+      </c>
+      <c r="C24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" t="n">
+        <v>17</v>
+      </c>
+      <c r="E24" t="n">
+        <v>13</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.764705882352941</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>94</v>
+      </c>
+      <c r="B25" t="s">
+        <v>105</v>
+      </c>
+      <c r="C25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" t="n">
+        <v>8</v>
+      </c>
+      <c r="E25" t="n">
+        <v>5</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>94</v>
+      </c>
+      <c r="B26" t="s">
+        <v>113</v>
+      </c>
+      <c r="C26" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" t="n">
+        <v>32</v>
+      </c>
+      <c r="E26" t="n">
+        <v>24</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>94</v>
+      </c>
+      <c r="B27" t="s">
+        <v>113</v>
+      </c>
+      <c r="C27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" t="n">
+        <v>21</v>
+      </c>
+      <c r="E27" t="n">
+        <v>14</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>94</v>
+      </c>
+      <c r="B28" t="s">
+        <v>113</v>
+      </c>
+      <c r="C28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" t="n">
+        <v>13</v>
+      </c>
+      <c r="E28" t="n">
+        <v>10</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.769230769230769</v>
+      </c>
+      <c r="G28" t="n">
+        <v>1</v>
+      </c>
+      <c r="H28" t="n">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E1" t="s">
+        <v>223</v>
+      </c>
+      <c r="F1" t="s">
+        <v>224</v>
+      </c>
+      <c r="G1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="n">
+        <v>20</v>
+      </c>
+      <c r="D2" t="n">
+        <v>16</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" t="n">
+        <v>31</v>
+      </c>
+      <c r="D5" t="n">
+        <v>7</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.225806451612903</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" t="n">
+        <v>71</v>
+      </c>
+      <c r="D6" t="n">
+        <v>3</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.0422535211267606</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" t="n">
+        <v>53</v>
+      </c>
+      <c r="D7" t="n">
+        <v>29</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.547169811320755</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C8" t="n">
+        <v>17</v>
+      </c>
+      <c r="D8" t="n">
+        <v>9</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.529411764705882</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C9" t="n">
+        <v>32</v>
+      </c>
+      <c r="D9" t="n">
+        <v>22</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.6875</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C10" t="n">
+        <v>66</v>
+      </c>
+      <c r="D10" t="n">
+        <v>48</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.727272727272727</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D1" t="s">
+        <v>223</v>
+      </c>
+      <c r="E1" t="s">
+        <v>224</v>
+      </c>
+      <c r="F1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="n">
+        <v>26</v>
+      </c>
+      <c r="C2" t="n">
+        <v>22</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.846153846153846</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" t="n">
+        <v>155</v>
+      </c>
+      <c r="C3" t="n">
+        <v>39</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.251612903225806</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" t="n">
+        <v>115</v>
+      </c>
+      <c r="C4" t="n">
+        <v>79</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.68695652173913</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>